<commit_message>
Late entries for 2025-12-08
</commit_message>
<xml_diff>
--- a/data/2025-12-08/SCW Weekly Comp 2025-12-08 (Responses).xlsx
+++ b/data/2025-12-08/SCW Weekly Comp 2025-12-08 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="294">
   <si>
     <t>Timestamp</t>
   </si>
@@ -860,6 +860,39 @@
   </si>
   <si>
     <t>5:18.00</t>
+  </si>
+  <si>
+    <t>Kristina Lim</t>
+  </si>
+  <si>
+    <t>2022LIMK02</t>
+  </si>
+  <si>
+    <t>Skewb</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/26073220195613492/?post_id=26156732813928896&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1604758584053522?post_id=1611637990032248&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1166515255682208/?post_id=1173324205001313&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>2:48.98</t>
+  </si>
+  <si>
+    <t>2:12.61</t>
+  </si>
+  <si>
+    <t>1:56.84</t>
+  </si>
+  <si>
+    <t>DNS</t>
+  </si>
+  <si>
+    <t>2:19.48</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1110,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:DF46" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:DF49" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="110">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Name" id="2"/>
@@ -3590,6 +3623,129 @@
         <v>131</v>
       </c>
     </row>
+    <row r="47" ht="22.5" customHeight="1">
+      <c r="A47" s="9">
+        <v>46017.04570372685</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="BO47" s="10">
+        <v>7.34</v>
+      </c>
+      <c r="BP47" s="10">
+        <v>5.69</v>
+      </c>
+      <c r="BQ47" s="10">
+        <v>8.4</v>
+      </c>
+      <c r="BR47" s="10">
+        <v>8.21</v>
+      </c>
+      <c r="BS47" s="10">
+        <v>8.14</v>
+      </c>
+      <c r="BT47" s="10">
+        <v>5.69</v>
+      </c>
+      <c r="BU47" s="10">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="48" ht="22.5" customHeight="1">
+      <c r="A48" s="9">
+        <v>46017.04747877315</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="H48" s="10">
+        <v>14.78</v>
+      </c>
+      <c r="I48" s="10">
+        <v>10.81</v>
+      </c>
+      <c r="J48" s="10">
+        <v>7.89</v>
+      </c>
+      <c r="K48" s="10">
+        <v>8.58</v>
+      </c>
+      <c r="L48" s="10">
+        <v>30.63</v>
+      </c>
+      <c r="M48" s="10">
+        <v>7.89</v>
+      </c>
+      <c r="N48" s="10">
+        <v>11.39</v>
+      </c>
+    </row>
+    <row r="49" ht="22.5" customHeight="1">
+      <c r="A49" s="9">
+        <v>46017.05572443287</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="V49" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="W49" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="X49" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y49" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="Z49" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="AA49" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB49" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
@@ -3637,10 +3793,13 @@
     <hyperlink r:id="rId43" ref="F44"/>
     <hyperlink r:id="rId44" ref="F45"/>
     <hyperlink r:id="rId45" ref="F46"/>
+    <hyperlink r:id="rId46" ref="F47"/>
+    <hyperlink r:id="rId47" ref="F48"/>
+    <hyperlink r:id="rId48" ref="F49"/>
   </hyperlinks>
-  <drawing r:id="rId46"/>
+  <drawing r:id="rId49"/>
   <tableParts count="1">
-    <tablePart r:id="rId48"/>
+    <tablePart r:id="rId51"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>